<commit_message>
fitted to my data
</commit_message>
<xml_diff>
--- a/raw/biomass.xlsx
+++ b/raw/biomass.xlsx
@@ -15,6 +15,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd HH:mm:ss UTC"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -52,11 +55,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -351,2500 +355,3226 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H73"/>
+  <dimension ref="A1:L73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="20.7109375" style="2" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>Harvest_date</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>Site</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Transect</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Location</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Tube_ID</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>harvest_w</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>dry_w</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>hyphal_weight</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Notes.x</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>bag_damage</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>correction</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>corrected_weight</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" s="2">
+        <v>45608</v>
+      </c>
+      <c r="B2" t="inlineStr">
         <is>
           <t>S34</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="C2" t="inlineStr">
         <is>
           <t>T1</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="D2" t="inlineStr">
         <is>
           <t>L3</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="E2" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>26.51</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>14.138</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>0.355</v>
       </c>
-      <c r="H2">
-        <v>0.3536634036144578</v>
+      <c r="J2">
+        <v>-0.06460843373493994</v>
+      </c>
+      <c r="K2">
+        <v>0.93539156626506</v>
+      </c>
+      <c r="L2">
+        <v>0.3320640060240963</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
+      <c r="A3" s="2">
+        <v>45608</v>
+      </c>
+      <c r="B3" t="inlineStr">
         <is>
           <t>S34</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="C3" t="inlineStr">
         <is>
           <t>T1</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="D3" t="inlineStr">
         <is>
           <t>L9</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="E3" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>25.75</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>16.492</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>0.868</v>
       </c>
-      <c r="H3">
-        <v>0.8150572289156628</v>
+      <c r="J3">
+        <v>-0.2418674698795182</v>
+      </c>
+      <c r="K3">
+        <v>0.7581325301204818</v>
+      </c>
+      <c r="L3">
+        <v>0.6580590361445782</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
+      <c r="A4" s="2">
+        <v>45608</v>
+      </c>
+      <c r="B4" t="inlineStr">
         <is>
           <t>S34</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="C4" t="inlineStr">
         <is>
           <t>T1</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="D4" t="inlineStr">
         <is>
           <t>L15</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="E4" t="inlineStr">
         <is>
           <t>3</t>
         </is>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>18.45</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>9.655000000000001</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>0.9370000000000001</v>
       </c>
-      <c r="H4">
-        <v>0.3647808734939759</v>
+      <c r="J4">
+        <v>0.2729668674698794</v>
+      </c>
+      <c r="K4">
+        <v>1.272966867469879</v>
+      </c>
+      <c r="L4">
+        <v>1.192769954819277</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
+      <c r="A5" s="2">
+        <v>45608</v>
+      </c>
+      <c r="B5" t="inlineStr">
         <is>
           <t>S34</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="C5" t="inlineStr">
         <is>
           <t>T1</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="D5" t="inlineStr">
         <is>
           <t>L33</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="E5" t="inlineStr">
         <is>
           <t>4</t>
         </is>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>26.22</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>18.083</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>0.701</v>
       </c>
-      <c r="H5">
-        <v>0.6830527108433735</v>
+      <c r="J5">
+        <v>-0.3616716867469879</v>
+      </c>
+      <c r="K5">
+        <v>0.6383283132530121</v>
+      </c>
+      <c r="L5">
+        <v>0.4474681475903615</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
+      <c r="A6" s="2">
+        <v>45608</v>
+      </c>
+      <c r="B6" t="inlineStr">
         <is>
           <t>S34</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="C6" t="inlineStr">
         <is>
           <t>T1</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="D6" t="inlineStr">
         <is>
           <t>L41</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
+      <c r="E6" t="inlineStr">
         <is>
           <t>5</t>
         </is>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>26.61</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>17.777</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>0.261</v>
       </c>
-      <c r="H6">
-        <v>0.2619826807228916</v>
+      <c r="J6">
+        <v>-0.3386295180722893</v>
+      </c>
+      <c r="K6">
+        <v>0.6613704819277106</v>
+      </c>
+      <c r="L6">
+        <v>0.1726176957831325</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
+      <c r="A7" s="2">
+        <v>45608</v>
+      </c>
+      <c r="B7" t="inlineStr">
         <is>
           <t>S34</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
+      <c r="C7" t="inlineStr">
         <is>
           <t>T1</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="D7" t="inlineStr">
         <is>
           <t>L47</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
+      <c r="E7" t="inlineStr">
         <is>
           <t>6</t>
         </is>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>25.71</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>15.443</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>0.44</v>
       </c>
-      <c r="H7">
-        <v>0.4118373493975905</v>
+      <c r="J7">
+        <v>-0.1628765060240965</v>
+      </c>
+      <c r="K7">
+        <v>0.8371234939759035</v>
+      </c>
+      <c r="L7">
+        <v>0.3683343373493975</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
+      <c r="A8" s="2">
+        <v>45608</v>
+      </c>
+      <c r="B8" t="inlineStr">
         <is>
           <t>S34</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
+      <c r="C8" t="inlineStr">
         <is>
           <t>T2</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
+      <c r="D8" t="inlineStr">
         <is>
           <t>L3</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
+      <c r="E8" t="inlineStr">
         <is>
           <t>7</t>
         </is>
       </c>
-      <c r="E8">
+      <c r="F8">
         <v>12.82</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>7.191</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>0.47</v>
       </c>
-      <c r="H8">
-        <v>-0.01628012048192768</v>
+      <c r="J8">
+        <v>0.4585090361445783</v>
+      </c>
+      <c r="K8">
+        <v>1.458509036144578</v>
+      </c>
+      <c r="L8">
+        <v>0.6854992469879517</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
+      <c r="A9" s="2">
+        <v>45608</v>
+      </c>
+      <c r="B9" t="inlineStr">
         <is>
           <t>S34</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
+      <c r="C9" t="inlineStr">
         <is>
           <t>T2</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="D9" t="inlineStr">
         <is>
           <t>L10</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
+      <c r="E9" t="inlineStr">
         <is>
           <t>8</t>
         </is>
       </c>
-      <c r="E9">
+      <c r="F9">
         <v>26.06</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>13.33</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>0.313</v>
       </c>
-      <c r="H9">
-        <v>0.3012153614457832</v>
+      <c r="J9">
+        <v>-0.003765060240963775</v>
+      </c>
+      <c r="K9">
+        <v>0.9962349397590362</v>
+      </c>
+      <c r="L9">
+        <v>0.3118215361445784</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
+      <c r="A10" s="2">
+        <v>45608</v>
+      </c>
+      <c r="B10" t="inlineStr">
         <is>
           <t>S34</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
+      <c r="C10" t="inlineStr">
         <is>
           <t>T2</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
+      <c r="D10" t="inlineStr">
         <is>
           <t>L16</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
+      <c r="E10" t="inlineStr">
         <is>
           <t>9</t>
         </is>
       </c>
-      <c r="E10">
+      <c r="F10">
         <v>13.66</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>7.589</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <v>0.167</v>
       </c>
-      <c r="H10">
-        <v>0.004778614457831336</v>
+      <c r="J10">
+        <v>0.428539156626506</v>
+      </c>
+      <c r="K10">
+        <v>1.428539156626506</v>
+      </c>
+      <c r="L10">
+        <v>0.2385660391566265</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
+      <c r="A11" s="2">
+        <v>45608</v>
+      </c>
+      <c r="B11" t="inlineStr">
         <is>
           <t>S34</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
+      <c r="C11" t="inlineStr">
         <is>
           <t>T2</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
+      <c r="D11" t="inlineStr">
         <is>
           <t>L31</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
+      <c r="E11" t="inlineStr">
         <is>
           <t>10</t>
         </is>
       </c>
-      <c r="E11">
+      <c r="F11">
         <v>26.68</v>
       </c>
-      <c r="F11">
+      <c r="G11">
         <v>17.504</v>
       </c>
-      <c r="G11">
+      <c r="H11">
         <v>0.631</v>
       </c>
-      <c r="H11">
-        <v>0.6367018072289158</v>
+      <c r="J11">
+        <v>-0.3180722891566267</v>
+      </c>
+      <c r="K11">
+        <v>0.6819277108433733</v>
+      </c>
+      <c r="L11">
+        <v>0.4302963855421686</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
+      <c r="A12" s="2">
+        <v>45608</v>
+      </c>
+      <c r="B12" t="inlineStr">
         <is>
           <t>S34</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
+      <c r="C12" t="inlineStr">
         <is>
           <t>T2</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
+      <c r="D12" t="inlineStr">
         <is>
           <t>L39</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
+      <c r="E12" t="inlineStr">
         <is>
           <t>11</t>
         </is>
       </c>
-      <c r="E12">
+      <c r="F12">
         <v>21.88</v>
       </c>
-      <c r="F12">
+      <c r="G12">
         <v>13.684</v>
       </c>
-      <c r="G12">
+      <c r="H12">
         <v>0.393</v>
       </c>
-      <c r="H12">
-        <v>0.2545030120481929</v>
+      <c r="J12">
+        <v>-0.03042168674698808</v>
+      </c>
+      <c r="K12">
+        <v>0.9695783132530119</v>
+      </c>
+      <c r="L12">
+        <v>0.3810442771084337</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr">
+      <c r="A13" s="2">
+        <v>45608</v>
+      </c>
+      <c r="B13" t="inlineStr">
         <is>
           <t>S34</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
+      <c r="C13" t="inlineStr">
         <is>
           <t>T2</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
+      <c r="D13" t="inlineStr">
         <is>
           <t>L47</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr">
+      <c r="E13" t="inlineStr">
         <is>
           <t>12</t>
         </is>
       </c>
-      <c r="E13">
+      <c r="F13">
         <v>26.44</v>
       </c>
-      <c r="F13">
+      <c r="G13">
         <v>17.468</v>
       </c>
-      <c r="G13">
+      <c r="H13">
         <v>0.425</v>
       </c>
-      <c r="H13">
-        <v>0.421159638554217</v>
+      <c r="J13">
+        <v>-0.3153614457831326</v>
+      </c>
+      <c r="K13">
+        <v>0.6846385542168674</v>
+      </c>
+      <c r="L13">
+        <v>0.2909713855421686</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="inlineStr">
+      <c r="A14" s="2">
+        <v>45608</v>
+      </c>
+      <c r="B14" t="inlineStr">
         <is>
           <t>S12</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
+      <c r="C14" t="inlineStr">
         <is>
           <t>T1</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr">
+      <c r="D14" t="inlineStr">
         <is>
           <t>L3</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr">
+      <c r="E14" t="inlineStr">
         <is>
           <t>13</t>
         </is>
       </c>
-      <c r="E14">
+      <c r="F14">
         <v>25.72</v>
       </c>
-      <c r="F14">
+      <c r="G14">
         <v>20.2</v>
       </c>
-      <c r="G14">
+      <c r="H14">
         <v>0.511</v>
       </c>
-      <c r="H14">
-        <v>0.4786777108433735</v>
+      <c r="J14">
+        <v>-0.5210843373493976</v>
+      </c>
+      <c r="K14">
+        <v>0.4789156626506024</v>
+      </c>
+      <c r="L14">
+        <v>0.2447259036144578</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="inlineStr">
+      <c r="A15" s="2">
+        <v>45608</v>
+      </c>
+      <c r="B15" t="inlineStr">
         <is>
           <t>S12</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr">
+      <c r="C15" t="inlineStr">
         <is>
           <t>T1</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr">
+      <c r="D15" t="inlineStr">
         <is>
           <t>L9</t>
         </is>
       </c>
-      <c r="D15" t="inlineStr">
+      <c r="E15" t="inlineStr">
         <is>
           <t>14</t>
         </is>
       </c>
-      <c r="E15">
+      <c r="F15">
         <v>26.51</v>
       </c>
-      <c r="F15">
+      <c r="G15">
         <v>20.9</v>
       </c>
-      <c r="G15">
+      <c r="H15">
         <v>0.819</v>
       </c>
-      <c r="H15">
-        <v>0.8159164156626507</v>
+      <c r="J15">
+        <v>-0.5737951807228915</v>
+      </c>
+      <c r="K15">
+        <v>0.4262048192771085</v>
+      </c>
+      <c r="L15">
+        <v>0.3490617469879518</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="inlineStr">
+      <c r="A16" s="2">
+        <v>45608</v>
+      </c>
+      <c r="B16" t="inlineStr">
         <is>
           <t>S12</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr">
+      <c r="C16" t="inlineStr">
         <is>
           <t>T1</t>
         </is>
       </c>
-      <c r="C16" t="inlineStr">
+      <c r="D16" t="inlineStr">
         <is>
           <t>L16</t>
         </is>
       </c>
-      <c r="D16" t="inlineStr">
+      <c r="E16" t="inlineStr">
         <is>
           <t>15</t>
         </is>
       </c>
-      <c r="E16">
+      <c r="F16">
         <v>22.28</v>
       </c>
-      <c r="F16">
+      <c r="G16">
         <v>15.99</v>
       </c>
-      <c r="G16">
+      <c r="H16">
         <v>0.5590000000000001</v>
       </c>
-      <c r="H16">
-        <v>0.3788403614457833</v>
+      <c r="J16">
+        <v>-0.2040662650602409</v>
+      </c>
+      <c r="K16">
+        <v>0.7959337349397591</v>
+      </c>
+      <c r="L16">
+        <v>0.4449269578313254</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="inlineStr">
+      <c r="A17" s="2">
+        <v>45608</v>
+      </c>
+      <c r="B17" t="inlineStr">
         <is>
           <t>S12</t>
         </is>
       </c>
-      <c r="B17" t="inlineStr">
+      <c r="C17" t="inlineStr">
         <is>
           <t>T1</t>
         </is>
       </c>
-      <c r="C17" t="inlineStr">
+      <c r="D17" t="inlineStr">
         <is>
           <t>L33</t>
         </is>
       </c>
-      <c r="D17" t="inlineStr">
+      <c r="E17" t="inlineStr">
         <is>
           <t>16</t>
         </is>
       </c>
-      <c r="E17">
+      <c r="F17">
         <v>26.63</v>
       </c>
-      <c r="F17">
+      <c r="G17">
         <v>22.38</v>
       </c>
-      <c r="G17">
+      <c r="H17">
         <v>0.389</v>
       </c>
-      <c r="H17">
-        <v>0.3910504518072291</v>
+      <c r="J17">
+        <v>-0.6852409638554217</v>
+      </c>
+      <c r="K17">
+        <v>0.3147590361445783</v>
+      </c>
+      <c r="L17">
+        <v>0.122441265060241</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="inlineStr">
+      <c r="A18" s="2">
+        <v>45608</v>
+      </c>
+      <c r="B18" t="inlineStr">
         <is>
           <t>S12</t>
         </is>
       </c>
-      <c r="B18" t="inlineStr">
+      <c r="C18" t="inlineStr">
         <is>
           <t>T1</t>
         </is>
       </c>
-      <c r="C18" t="inlineStr">
+      <c r="D18" t="inlineStr">
         <is>
           <t>L39</t>
         </is>
       </c>
-      <c r="D18" t="inlineStr">
+      <c r="E18" t="inlineStr">
         <is>
           <t>17</t>
         </is>
       </c>
-      <c r="E18">
+      <c r="F18">
         <v>16.21</v>
       </c>
-      <c r="F18">
+      <c r="G18">
         <v>12.57</v>
       </c>
-      <c r="G18">
+      <c r="H18">
         <v>0.65</v>
       </c>
-      <c r="H18">
-        <v>0.1434111445783133</v>
+      <c r="J18">
+        <v>0.05346385542168668</v>
+      </c>
+      <c r="K18">
+        <v>1.053463855421687</v>
+      </c>
+      <c r="L18">
+        <v>0.6847515060240963</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="inlineStr">
+      <c r="A19" s="2">
+        <v>45608</v>
+      </c>
+      <c r="B19" t="inlineStr">
         <is>
           <t>S12</t>
         </is>
       </c>
-      <c r="B19" t="inlineStr">
+      <c r="C19" t="inlineStr">
         <is>
           <t>T1</t>
         </is>
       </c>
-      <c r="C19" t="inlineStr">
+      <c r="D19" t="inlineStr">
         <is>
           <t>L47</t>
         </is>
       </c>
-      <c r="D19" t="inlineStr">
+      <c r="E19" t="inlineStr">
         <is>
           <t>18</t>
         </is>
       </c>
-      <c r="E19">
+      <c r="F19">
         <v>25.35</v>
       </c>
-      <c r="F19">
+      <c r="G19">
         <v>22.27</v>
       </c>
-      <c r="G19">
+      <c r="H19">
         <v>0.907</v>
       </c>
-      <c r="H19">
-        <v>0.8243591867469882</v>
+      <c r="J19">
+        <v>-0.6769578313253013</v>
+      </c>
+      <c r="K19">
+        <v>0.3230421686746987</v>
+      </c>
+      <c r="L19">
+        <v>0.2929992469879517</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="inlineStr">
+      <c r="A20" s="2">
+        <v>45608</v>
+      </c>
+      <c r="B20" t="inlineStr">
         <is>
           <t>S12</t>
         </is>
       </c>
-      <c r="B20" t="inlineStr">
+      <c r="C20" t="inlineStr">
         <is>
           <t>T2</t>
         </is>
       </c>
-      <c r="C20" t="inlineStr">
+      <c r="D20" t="inlineStr">
         <is>
           <t>L3</t>
         </is>
       </c>
-      <c r="D20" t="inlineStr">
+      <c r="E20" t="inlineStr">
         <is>
           <t>19</t>
         </is>
       </c>
-      <c r="E20">
+      <c r="F20">
         <v>22.63</v>
       </c>
-      <c r="F20">
+      <c r="G20">
         <v>8.800000000000001</v>
       </c>
-      <c r="G20">
+      <c r="H20">
         <v>0.656</v>
       </c>
-      <c r="H20">
-        <v>0.4618674698795183</v>
+      <c r="J20">
+        <v>0.3373493975903614</v>
+      </c>
+      <c r="K20">
+        <v>1.337349397590361</v>
+      </c>
+      <c r="L20">
+        <v>0.8773012048192771</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="inlineStr">
+      <c r="A21" s="2">
+        <v>45608</v>
+      </c>
+      <c r="B21" t="inlineStr">
         <is>
           <t>S12</t>
         </is>
       </c>
-      <c r="B21" t="inlineStr">
+      <c r="C21" t="inlineStr">
         <is>
           <t>T2</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr">
+      <c r="D21" t="inlineStr">
         <is>
           <t>L9</t>
         </is>
       </c>
-      <c r="D21" t="inlineStr">
+      <c r="E21" t="inlineStr">
         <is>
           <t>20</t>
         </is>
       </c>
-      <c r="E21">
+      <c r="F21">
         <v>20.81</v>
       </c>
-      <c r="F21">
+      <c r="G21">
         <v>16.3</v>
       </c>
-      <c r="G21">
+      <c r="H21">
         <v>1.088</v>
       </c>
-      <c r="H21">
-        <v>0.6169156626506027</v>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>(White fungus around)</t>
+        </is>
+      </c>
+      <c r="J21">
+        <v>-0.2274096385542167</v>
+      </c>
+      <c r="K21">
+        <v>0.7725903614457833</v>
+      </c>
+      <c r="L21">
+        <v>0.8405783132530122</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" t="inlineStr">
+      <c r="A22" s="2">
+        <v>45608</v>
+      </c>
+      <c r="B22" t="inlineStr">
         <is>
           <t>S12</t>
         </is>
       </c>
-      <c r="B22" t="inlineStr">
+      <c r="C22" t="inlineStr">
         <is>
           <t>T2</t>
         </is>
       </c>
-      <c r="C22" t="inlineStr">
+      <c r="D22" t="inlineStr">
         <is>
           <t>L16</t>
         </is>
       </c>
-      <c r="D22" t="inlineStr">
+      <c r="E22" t="inlineStr">
         <is>
           <t>21</t>
         </is>
       </c>
-      <c r="E22">
+      <c r="F22">
         <v>22.64</v>
       </c>
-      <c r="F22">
+      <c r="G22">
         <v>17.515</v>
       </c>
-      <c r="G22">
+      <c r="H22">
         <v>0.311</v>
       </c>
-      <c r="H22">
-        <v>0.2191987951807229</v>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>D-Mod</t>
+        </is>
+      </c>
+      <c r="J22">
+        <v>-0.3189006024096386</v>
+      </c>
+      <c r="K22">
+        <v>0.6810993975903614</v>
+      </c>
+      <c r="L22">
+        <v>0.2118219126506024</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" t="inlineStr">
+      <c r="A23" s="2">
+        <v>45608</v>
+      </c>
+      <c r="B23" t="inlineStr">
         <is>
           <t>S12</t>
         </is>
       </c>
-      <c r="B23" t="inlineStr">
+      <c r="C23" t="inlineStr">
         <is>
           <t>T2</t>
         </is>
       </c>
-      <c r="C23" t="inlineStr">
+      <c r="D23" t="inlineStr">
         <is>
           <t>L33</t>
         </is>
       </c>
-      <c r="D23" t="inlineStr">
+      <c r="E23" t="inlineStr">
         <is>
           <t>22</t>
         </is>
       </c>
-      <c r="E23">
+      <c r="F23">
         <v>26.62</v>
       </c>
-      <c r="F23">
+      <c r="G23">
         <v>20.97</v>
       </c>
-      <c r="G23">
+      <c r="H23">
         <v>0.2</v>
       </c>
-      <c r="H23">
-        <v>0.2009036144578313</v>
+      <c r="J23">
+        <v>-0.5790662650602409</v>
+      </c>
+      <c r="K23">
+        <v>0.4209337349397591</v>
+      </c>
+      <c r="L23">
+        <v>0.08418674698795181</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" t="inlineStr">
+      <c r="A24" s="2">
+        <v>45608</v>
+      </c>
+      <c r="B24" t="inlineStr">
         <is>
           <t>S12</t>
         </is>
       </c>
-      <c r="B24" t="inlineStr">
+      <c r="C24" t="inlineStr">
         <is>
           <t>T2</t>
         </is>
       </c>
-      <c r="C24" t="inlineStr">
+      <c r="D24" t="inlineStr">
         <is>
           <t>L39</t>
         </is>
       </c>
-      <c r="D24" t="inlineStr">
+      <c r="E24" t="inlineStr">
         <is>
           <t>23</t>
         </is>
       </c>
-      <c r="E24">
+      <c r="F24">
         <v>14.5</v>
       </c>
-      <c r="F24">
+      <c r="G24">
         <v>10.56</v>
       </c>
-      <c r="G24">
+      <c r="H24">
         <v>0.8070000000000001</v>
       </c>
-      <c r="H24">
-        <v>0.07413704819277113</v>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>D-Major</t>
+        </is>
+      </c>
+      <c r="J24">
+        <v>0.2048192771084337</v>
+      </c>
+      <c r="K24">
+        <v>1.204819277108434</v>
+      </c>
+      <c r="L24">
+        <v>0.9722891566265059</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" t="inlineStr">
+      <c r="A25" s="2">
+        <v>45608</v>
+      </c>
+      <c r="B25" t="inlineStr">
         <is>
           <t>S12</t>
         </is>
       </c>
-      <c r="B25" t="inlineStr">
+      <c r="C25" t="inlineStr">
         <is>
           <t>T2</t>
         </is>
       </c>
-      <c r="C25" t="inlineStr">
+      <c r="D25" t="inlineStr">
         <is>
           <t>L47</t>
         </is>
       </c>
-      <c r="D25" t="inlineStr">
+      <c r="E25" t="inlineStr">
         <is>
           <t>24</t>
         </is>
       </c>
-      <c r="E25">
+      <c r="F25">
         <v>22.85</v>
       </c>
-      <c r="F25">
+      <c r="G25">
         <v>17.59</v>
       </c>
-      <c r="G25">
+      <c r="H25">
         <v>1</v>
       </c>
-      <c r="H25">
-        <v>0.7206325301204821</v>
+      <c r="J25">
+        <v>-0.3245481927710844</v>
+      </c>
+      <c r="K25">
+        <v>0.6754518072289156</v>
+      </c>
+      <c r="L25">
+        <v>0.6754518072289156</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" t="inlineStr">
+      <c r="A26" s="2">
+        <v>45608</v>
+      </c>
+      <c r="B26" t="inlineStr">
         <is>
           <t>S10</t>
         </is>
       </c>
-      <c r="B26" t="inlineStr">
+      <c r="C26" t="inlineStr">
         <is>
           <t>T1</t>
         </is>
       </c>
-      <c r="C26" t="inlineStr">
+      <c r="D26" t="inlineStr">
         <is>
           <t>L3</t>
         </is>
       </c>
-      <c r="D26" t="inlineStr">
+      <c r="E26" t="inlineStr">
         <is>
           <t>25</t>
         </is>
       </c>
-      <c r="E26">
+      <c r="F26">
         <v>25.67</v>
       </c>
-      <c r="F26">
+      <c r="G26">
         <v>0</v>
       </c>
-      <c r="G26">
+      <c r="H26">
         <v>0.626</v>
       </c>
-      <c r="H26">
-        <v>0.5840466867469881</v>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>NON recoverable dry weight (error in the oven)</t>
+        </is>
+      </c>
+      <c r="J26">
+        <v>1</v>
+      </c>
+      <c r="K26">
+        <v>2</v>
+      </c>
+      <c r="L26">
+        <v>1.252</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" t="inlineStr">
+      <c r="A27" s="2">
+        <v>45608</v>
+      </c>
+      <c r="B27" t="inlineStr">
         <is>
           <t>S10</t>
         </is>
       </c>
-      <c r="B27" t="inlineStr">
+      <c r="C27" t="inlineStr">
         <is>
           <t>T1</t>
         </is>
       </c>
-      <c r="C27" t="inlineStr">
+      <c r="D27" t="inlineStr">
         <is>
           <t>L10</t>
         </is>
       </c>
-      <c r="D27" t="inlineStr">
+      <c r="E27" t="inlineStr">
         <is>
           <t>26</t>
         </is>
       </c>
-      <c r="E27">
+      <c r="F27">
         <v>22.26</v>
       </c>
-      <c r="F27">
+      <c r="G27">
         <v>11.35</v>
       </c>
-      <c r="G27">
+      <c r="H27">
         <v>0.987</v>
       </c>
-      <c r="H27">
-        <v>0.6674141566265059</v>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>recovered from oven error</t>
+        </is>
+      </c>
+      <c r="J27">
+        <v>0.1453313253012048</v>
+      </c>
+      <c r="K27">
+        <v>1.145331325301205</v>
+      </c>
+      <c r="L27">
+        <v>1.130442018072289</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" t="inlineStr">
+      <c r="A28" s="2">
+        <v>45608</v>
+      </c>
+      <c r="B28" t="inlineStr">
         <is>
           <t>S10</t>
         </is>
       </c>
-      <c r="B28" t="inlineStr">
+      <c r="C28" t="inlineStr">
         <is>
           <t>T1</t>
         </is>
       </c>
-      <c r="C28" t="inlineStr">
+      <c r="D28" t="inlineStr">
         <is>
           <t>L16</t>
         </is>
       </c>
-      <c r="D28" t="inlineStr">
+      <c r="E28" t="inlineStr">
         <is>
           <t>27</t>
         </is>
       </c>
-      <c r="E28">
+      <c r="F28">
         <v>23.22</v>
       </c>
-      <c r="F28">
+      <c r="G28">
         <v>12.65</v>
       </c>
-      <c r="G28">
+      <c r="H28">
         <v>0.766</v>
       </c>
-      <c r="H28">
-        <v>0.5733463855421687</v>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>D-Minor</t>
+        </is>
+      </c>
+      <c r="J28">
+        <v>0.04743975903614451</v>
+      </c>
+      <c r="K28">
+        <v>1.047439759036145</v>
+      </c>
+      <c r="L28">
+        <v>0.8023388554216868</v>
       </c>
     </row>
     <row r="29">
-      <c r="A29" t="inlineStr">
+      <c r="A29" s="2">
+        <v>45608</v>
+      </c>
+      <c r="B29" t="inlineStr">
         <is>
           <t>S10</t>
         </is>
       </c>
-      <c r="B29" t="inlineStr">
+      <c r="C29" t="inlineStr">
         <is>
           <t>T1</t>
         </is>
       </c>
-      <c r="C29" t="inlineStr">
+      <c r="D29" t="inlineStr">
         <is>
           <t>L33</t>
         </is>
       </c>
-      <c r="D29" t="inlineStr">
+      <c r="E29" t="inlineStr">
         <is>
           <t>28</t>
         </is>
       </c>
-      <c r="E29">
+      <c r="F29">
         <v>22.32</v>
       </c>
-      <c r="F29">
+      <c r="G29">
         <v>11.53</v>
       </c>
-      <c r="G29">
+      <c r="H29">
         <v>0.667</v>
       </c>
-      <c r="H29">
-        <v>0.4540421686746989</v>
+      <c r="J29">
+        <v>0.1317771084337349</v>
+      </c>
+      <c r="K29">
+        <v>1.131777108433735</v>
+      </c>
+      <c r="L29">
+        <v>0.7548953313253012</v>
       </c>
     </row>
     <row r="30">
-      <c r="A30" t="inlineStr">
+      <c r="A30" s="2">
+        <v>45608</v>
+      </c>
+      <c r="B30" t="inlineStr">
         <is>
           <t>S10</t>
         </is>
       </c>
-      <c r="B30" t="inlineStr">
+      <c r="C30" t="inlineStr">
         <is>
           <t>T1</t>
         </is>
       </c>
-      <c r="C30" t="inlineStr">
+      <c r="D30" t="inlineStr">
         <is>
           <t>L39</t>
         </is>
       </c>
-      <c r="D30" t="inlineStr">
+      <c r="E30" t="inlineStr">
         <is>
           <t>29</t>
         </is>
       </c>
-      <c r="E30">
+      <c r="F30">
         <v>22.98</v>
       </c>
-      <c r="F30">
+      <c r="G30">
         <v>11.93</v>
       </c>
-      <c r="G30">
+      <c r="H30">
         <v>2.239</v>
       </c>
-      <c r="H30">
-        <v>1.635414156626506</v>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>D-Minor</t>
+        </is>
+      </c>
+      <c r="J30">
+        <v>0.1016566265060241</v>
+      </c>
+      <c r="K30">
+        <v>1.101656626506024</v>
+      </c>
+      <c r="L30">
+        <v>2.466609186746988</v>
       </c>
     </row>
     <row r="31">
-      <c r="A31" t="inlineStr">
+      <c r="A31" s="2">
+        <v>45608</v>
+      </c>
+      <c r="B31" t="inlineStr">
         <is>
           <t>S10</t>
         </is>
       </c>
-      <c r="B31" t="inlineStr">
+      <c r="C31" t="inlineStr">
         <is>
           <t>T1</t>
         </is>
       </c>
-      <c r="C31" t="inlineStr">
+      <c r="D31" t="inlineStr">
         <is>
           <t>L47</t>
         </is>
       </c>
-      <c r="D31" t="inlineStr">
+      <c r="E31" t="inlineStr">
         <is>
           <t>30</t>
         </is>
       </c>
-      <c r="E31">
+      <c r="F31">
         <v>23.19</v>
       </c>
-      <c r="F31">
+      <c r="G31">
         <v>12.07</v>
       </c>
-      <c r="G31">
+      <c r="H31">
         <v>1.257</v>
       </c>
-      <c r="H31">
-        <v>0.9380173192771083</v>
+      <c r="J31">
+        <v>0.09111445783132524</v>
+      </c>
+      <c r="K31">
+        <v>1.091114457831325</v>
+      </c>
+      <c r="L31">
+        <v>1.371530873493976</v>
       </c>
     </row>
     <row r="32">
-      <c r="A32" t="inlineStr">
+      <c r="A32" s="2">
+        <v>45608</v>
+      </c>
+      <c r="B32" t="inlineStr">
         <is>
           <t>S10</t>
         </is>
       </c>
-      <c r="B32" t="inlineStr">
+      <c r="C32" t="inlineStr">
         <is>
           <t>T2</t>
         </is>
       </c>
-      <c r="C32" t="inlineStr">
+      <c r="D32" t="inlineStr">
         <is>
           <t>L3</t>
         </is>
       </c>
-      <c r="D32" t="inlineStr">
+      <c r="E32" t="inlineStr">
         <is>
           <t>31</t>
         </is>
       </c>
-      <c r="E32">
+      <c r="F32">
         <v>19.4</v>
       </c>
-      <c r="F32">
+      <c r="G32">
         <v>10.01</v>
       </c>
-      <c r="G32">
+      <c r="H32">
         <v>0.354</v>
       </c>
-      <c r="H32">
-        <v>0.1631385542168675</v>
+      <c r="J32">
+        <v>0.2462349397590361</v>
+      </c>
+      <c r="K32">
+        <v>1.246234939759036</v>
+      </c>
+      <c r="L32">
+        <v>0.4411671686746988</v>
       </c>
     </row>
     <row r="33">
-      <c r="A33" t="inlineStr">
+      <c r="A33" s="2">
+        <v>45608</v>
+      </c>
+      <c r="B33" t="inlineStr">
         <is>
           <t>S10</t>
         </is>
       </c>
-      <c r="B33" t="inlineStr">
+      <c r="C33" t="inlineStr">
         <is>
           <t>T2</t>
         </is>
       </c>
-      <c r="C33" t="inlineStr">
+      <c r="D33" t="inlineStr">
         <is>
           <t>L10</t>
         </is>
       </c>
-      <c r="D33" t="inlineStr">
+      <c r="E33" t="inlineStr">
         <is>
           <t>32</t>
         </is>
       </c>
-      <c r="E33">
+      <c r="F33">
         <v>23.31</v>
       </c>
-      <c r="F33">
+      <c r="G33">
         <v>12.1</v>
       </c>
-      <c r="G33">
+      <c r="H33">
         <v>1.82</v>
       </c>
-      <c r="H33">
-        <v>1.374593373493976</v>
+      <c r="J33">
+        <v>0.08885542168674697</v>
+      </c>
+      <c r="K33">
+        <v>1.088855421686747</v>
+      </c>
+      <c r="L33">
+        <v>1.98171686746988</v>
       </c>
     </row>
     <row r="34">
-      <c r="A34" t="inlineStr">
+      <c r="A34" s="2">
+        <v>45608</v>
+      </c>
+      <c r="B34" t="inlineStr">
         <is>
           <t>S10</t>
         </is>
       </c>
-      <c r="B34" t="inlineStr">
+      <c r="C34" t="inlineStr">
         <is>
           <t>T2</t>
         </is>
       </c>
-      <c r="C34" t="inlineStr">
+      <c r="D34" t="inlineStr">
         <is>
           <t>L15</t>
         </is>
       </c>
-      <c r="D34" t="inlineStr">
+      <c r="E34" t="inlineStr">
         <is>
           <t>33</t>
         </is>
       </c>
-      <c r="E34">
+      <c r="F34">
         <v>22.95</v>
       </c>
-      <c r="F34">
+      <c r="G34">
         <v>12.01</v>
       </c>
-      <c r="G34">
+      <c r="H34">
         <v>2.32</v>
       </c>
-      <c r="H34">
-        <v>1.689337349397591</v>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>D-Minor</t>
+        </is>
+      </c>
+      <c r="J34">
+        <v>0.0956325301204819</v>
+      </c>
+      <c r="K34">
+        <v>1.095632530120482</v>
+      </c>
+      <c r="L34">
+        <v>2.541867469879518</v>
       </c>
     </row>
     <row r="35">
-      <c r="A35" t="inlineStr">
+      <c r="A35" s="2">
+        <v>45608</v>
+      </c>
+      <c r="B35" t="inlineStr">
         <is>
           <t>S10</t>
         </is>
       </c>
-      <c r="B35" t="inlineStr">
+      <c r="C35" t="inlineStr">
         <is>
           <t>T2</t>
         </is>
       </c>
-      <c r="C35" t="inlineStr">
+      <c r="D35" t="inlineStr">
         <is>
           <t>L33</t>
         </is>
       </c>
-      <c r="D35" t="inlineStr">
+      <c r="E35" t="inlineStr">
         <is>
           <t>34</t>
         </is>
       </c>
-      <c r="E35">
+      <c r="F35">
         <v>26.43</v>
       </c>
-      <c r="F35">
+      <c r="G35">
         <v>13.7</v>
       </c>
-      <c r="G35">
+      <c r="H35">
         <v>0.676</v>
       </c>
-      <c r="H35">
-        <v>0.669382530120482</v>
+      <c r="J35">
+        <v>-0.03162650602409638</v>
+      </c>
+      <c r="K35">
+        <v>0.9683734939759037</v>
+      </c>
+      <c r="L35">
+        <v>0.6546204819277109</v>
       </c>
     </row>
     <row r="36">
-      <c r="A36" t="inlineStr">
+      <c r="A36" s="2">
+        <v>45608</v>
+      </c>
+      <c r="B36" t="inlineStr">
         <is>
           <t>S10</t>
         </is>
       </c>
-      <c r="B36" t="inlineStr">
+      <c r="C36" t="inlineStr">
         <is>
           <t>T2</t>
         </is>
       </c>
-      <c r="C36" t="inlineStr">
+      <c r="D36" t="inlineStr">
         <is>
           <t>L39</t>
         </is>
       </c>
-      <c r="D36" t="inlineStr">
+      <c r="E36" t="inlineStr">
         <is>
           <t>35</t>
         </is>
       </c>
-      <c r="E36">
+      <c r="F36">
         <v>25.87</v>
       </c>
-      <c r="F36">
+      <c r="G36">
         <v>13.68</v>
       </c>
-      <c r="G36">
+      <c r="H36">
         <v>0.457</v>
       </c>
-      <c r="H36">
-        <v>0.4332552710843373</v>
+      <c r="J36">
+        <v>-0.03012048192771087</v>
+      </c>
+      <c r="K36">
+        <v>0.9698795180722891</v>
+      </c>
+      <c r="L36">
+        <v>0.4432349397590362</v>
       </c>
     </row>
     <row r="37">
-      <c r="A37" t="inlineStr">
+      <c r="A37" s="2">
+        <v>45608</v>
+      </c>
+      <c r="B37" t="inlineStr">
         <is>
           <t>S10</t>
         </is>
       </c>
-      <c r="B37" t="inlineStr">
+      <c r="C37" t="inlineStr">
         <is>
           <t>T2</t>
         </is>
       </c>
-      <c r="C37" t="inlineStr">
+      <c r="D37" t="inlineStr">
         <is>
           <t>L47</t>
         </is>
       </c>
-      <c r="D37" t="inlineStr">
+      <c r="E37" t="inlineStr">
         <is>
           <t>36</t>
         </is>
       </c>
-      <c r="E37">
+      <c r="F37">
         <v>15.81</v>
       </c>
-      <c r="F37">
+      <c r="G37">
         <v>8.18</v>
       </c>
-      <c r="G37">
+      <c r="H37">
         <v>0.641</v>
       </c>
-      <c r="H37">
-        <v>0.1221182228915663</v>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>D-Minor</t>
+        </is>
+      </c>
+      <c r="J37">
+        <v>0.3840361445783133</v>
+      </c>
+      <c r="K37">
+        <v>1.384036144578313</v>
+      </c>
+      <c r="L37">
+        <v>0.8871671686746989</v>
       </c>
     </row>
     <row r="38">
-      <c r="A38" t="inlineStr">
+      <c r="A38" s="2">
+        <v>45608</v>
+      </c>
+      <c r="B38" t="inlineStr">
         <is>
           <t>S26</t>
         </is>
       </c>
-      <c r="B38" t="inlineStr">
+      <c r="C38" t="inlineStr">
         <is>
           <t>T1</t>
         </is>
       </c>
-      <c r="C38" t="inlineStr">
+      <c r="D38" t="inlineStr">
         <is>
           <t>L3</t>
         </is>
       </c>
-      <c r="D38" t="inlineStr">
+      <c r="E38" t="inlineStr">
         <is>
           <t>37</t>
         </is>
       </c>
-      <c r="E38">
+      <c r="F38">
         <v>20.48</v>
       </c>
-      <c r="F38">
+      <c r="G38">
         <v>10.37</v>
       </c>
-      <c r="G38">
+      <c r="H38">
         <v>0.341</v>
       </c>
-      <c r="H38">
-        <v>0.1848795180722892</v>
+      <c r="J38">
+        <v>0.2191265060240963</v>
+      </c>
+      <c r="K38">
+        <v>1.219126506024096</v>
+      </c>
+      <c r="L38">
+        <v>0.4157221385542169</v>
       </c>
     </row>
     <row r="39">
-      <c r="A39" t="inlineStr">
+      <c r="A39" s="2">
+        <v>45608</v>
+      </c>
+      <c r="B39" t="inlineStr">
         <is>
           <t>S26</t>
         </is>
       </c>
-      <c r="B39" t="inlineStr">
+      <c r="C39" t="inlineStr">
         <is>
           <t>T1</t>
         </is>
       </c>
-      <c r="C39" t="inlineStr">
+      <c r="D39" t="inlineStr">
         <is>
           <t>L10</t>
         </is>
       </c>
-      <c r="D39" t="inlineStr">
+      <c r="E39" t="inlineStr">
         <is>
           <t>38</t>
         </is>
       </c>
-      <c r="E39">
+      <c r="F39">
         <v>25.08</v>
       </c>
-      <c r="F39">
+      <c r="G39">
         <v>13.01</v>
       </c>
-      <c r="G39">
+      <c r="H39">
         <v>1.874</v>
       </c>
-      <c r="H39">
-        <v>1.665150602409639</v>
+      <c r="J39">
+        <v>0.02033132530120479</v>
+      </c>
+      <c r="K39">
+        <v>1.020331325301205</v>
+      </c>
+      <c r="L39">
+        <v>1.912100903614458</v>
       </c>
     </row>
     <row r="40">
-      <c r="A40" t="inlineStr">
+      <c r="A40" s="2">
+        <v>45608</v>
+      </c>
+      <c r="B40" t="inlineStr">
         <is>
           <t>S26</t>
         </is>
       </c>
-      <c r="B40" t="inlineStr">
+      <c r="C40" t="inlineStr">
         <is>
           <t>T1</t>
         </is>
       </c>
-      <c r="C40" t="inlineStr">
+      <c r="D40" t="inlineStr">
         <is>
           <t>L16</t>
         </is>
       </c>
-      <c r="D40" t="inlineStr">
+      <c r="E40" t="inlineStr">
         <is>
           <t>39</t>
         </is>
       </c>
-      <c r="E40">
+      <c r="F40">
         <v>26</v>
       </c>
-      <c r="F40">
+      <c r="G40">
         <v>13.49</v>
       </c>
-      <c r="G40">
+      <c r="H40">
         <v>0.39</v>
       </c>
-      <c r="H40">
-        <v>0.3735542168674699</v>
+      <c r="J40">
+        <v>-0.01581325301204812</v>
+      </c>
+      <c r="K40">
+        <v>0.9841867469879518</v>
+      </c>
+      <c r="L40">
+        <v>0.3838328313253012</v>
       </c>
     </row>
     <row r="41">
-      <c r="A41" t="inlineStr">
+      <c r="A41" s="2">
+        <v>45608</v>
+      </c>
+      <c r="B41" t="inlineStr">
         <is>
           <t>S26</t>
         </is>
       </c>
-      <c r="B41" t="inlineStr">
+      <c r="C41" t="inlineStr">
         <is>
           <t>T1</t>
         </is>
       </c>
-      <c r="C41" t="inlineStr">
+      <c r="D41" t="inlineStr">
         <is>
           <t>L33</t>
         </is>
       </c>
-      <c r="D41" t="inlineStr">
+      <c r="E41" t="inlineStr">
         <is>
           <t>40</t>
         </is>
       </c>
-      <c r="E41">
+      <c r="F41">
         <v>25.3</v>
       </c>
-      <c r="F41">
+      <c r="G41">
         <v>13.25</v>
       </c>
-      <c r="G41">
+      <c r="H41">
         <v>0.89</v>
       </c>
-      <c r="H41">
-        <v>0.8055572289156628</v>
+      <c r="J41">
+        <v>0.002259036144578265</v>
+      </c>
+      <c r="K41">
+        <v>1.002259036144578</v>
+      </c>
+      <c r="L41">
+        <v>0.8920105421686746</v>
       </c>
     </row>
     <row r="42">
-      <c r="A42" t="inlineStr">
+      <c r="A42" s="2">
+        <v>45608</v>
+      </c>
+      <c r="B42" t="inlineStr">
         <is>
           <t>S26</t>
         </is>
       </c>
-      <c r="B42" t="inlineStr">
+      <c r="C42" t="inlineStr">
         <is>
           <t>T1</t>
         </is>
       </c>
-      <c r="C42" t="inlineStr">
+      <c r="D42" t="inlineStr">
         <is>
           <t>L39</t>
         </is>
       </c>
-      <c r="D42" t="inlineStr">
+      <c r="E42" t="inlineStr">
         <is>
           <t>41</t>
         </is>
       </c>
-      <c r="E42">
+      <c r="F42">
         <v>19.9</v>
       </c>
-      <c r="F42">
+      <c r="G42">
         <v>10.2</v>
       </c>
-      <c r="G42">
+      <c r="H42">
         <v>0.743</v>
       </c>
-      <c r="H42">
-        <v>0.3703810240963855</v>
+      <c r="J42">
+        <v>0.2319277108433735</v>
+      </c>
+      <c r="K42">
+        <v>1.231927710843373</v>
+      </c>
+      <c r="L42">
+        <v>0.9153222891566265</v>
       </c>
     </row>
     <row r="43">
-      <c r="A43" t="inlineStr">
+      <c r="A43" s="2">
+        <v>45608</v>
+      </c>
+      <c r="B43" t="inlineStr">
         <is>
           <t>S26</t>
         </is>
       </c>
-      <c r="B43" t="inlineStr">
+      <c r="C43" t="inlineStr">
         <is>
           <t>T1</t>
         </is>
       </c>
-      <c r="C43" t="inlineStr">
+      <c r="D43" t="inlineStr">
         <is>
           <t>L47</t>
         </is>
       </c>
-      <c r="D43" t="inlineStr">
+      <c r="E43" t="inlineStr">
         <is>
           <t>42</t>
         </is>
       </c>
-      <c r="E43">
+      <c r="F43">
         <v>24</v>
       </c>
-      <c r="F43">
+      <c r="G43">
         <v>12.63</v>
       </c>
-      <c r="G43">
+      <c r="H43">
         <v>0.86</v>
       </c>
-      <c r="H43">
-        <v>0.6942168674698795</v>
+      <c r="J43">
+        <v>0.04894578313253015</v>
+      </c>
+      <c r="K43">
+        <v>1.04894578313253</v>
+      </c>
+      <c r="L43">
+        <v>0.9020933734939759</v>
       </c>
     </row>
     <row r="44">
-      <c r="A44" t="inlineStr">
+      <c r="A44" s="2">
+        <v>45608</v>
+      </c>
+      <c r="B44" t="inlineStr">
         <is>
           <t>S26</t>
         </is>
       </c>
-      <c r="B44" t="inlineStr">
+      <c r="C44" t="inlineStr">
         <is>
           <t>T2</t>
         </is>
       </c>
-      <c r="C44" t="inlineStr">
+      <c r="D44" t="inlineStr">
         <is>
           <t>L3</t>
         </is>
       </c>
-      <c r="D44" t="inlineStr">
+      <c r="E44" t="inlineStr">
         <is>
           <t>43</t>
         </is>
       </c>
-      <c r="E44">
+      <c r="F44">
         <v>23.45</v>
       </c>
-      <c r="F44">
+      <c r="G44">
         <v>12.14</v>
       </c>
-      <c r="G44">
+      <c r="H44">
         <v>0.91</v>
       </c>
-      <c r="H44">
-        <v>0.696890060240964</v>
+      <c r="J44">
+        <v>0.08584337349397582</v>
+      </c>
+      <c r="K44">
+        <v>1.085843373493976</v>
+      </c>
+      <c r="L44">
+        <v>0.9881174698795181</v>
       </c>
     </row>
     <row r="45">
-      <c r="A45" t="inlineStr">
+      <c r="A45" s="2">
+        <v>45608</v>
+      </c>
+      <c r="B45" t="inlineStr">
         <is>
           <t>S26</t>
         </is>
       </c>
-      <c r="B45" t="inlineStr">
+      <c r="C45" t="inlineStr">
         <is>
           <t>T2</t>
         </is>
       </c>
-      <c r="C45" t="inlineStr">
+      <c r="D45" t="inlineStr">
         <is>
           <t>L10</t>
         </is>
       </c>
-      <c r="D45" t="inlineStr">
+      <c r="E45" t="inlineStr">
         <is>
           <t>44</t>
         </is>
       </c>
-      <c r="E45">
+      <c r="F45">
         <v>12.56</v>
       </c>
-      <c r="F45">
+      <c r="G45">
         <v>6.46</v>
       </c>
-      <c r="G45">
+      <c r="H45">
         <v>0.28</v>
       </c>
-      <c r="H45">
-        <v>-0.01518072289156624</v>
+      <c r="J45">
+        <v>0.5135542168674698</v>
+      </c>
+      <c r="K45">
+        <v>1.51355421686747</v>
+      </c>
+      <c r="L45">
+        <v>0.4237951807228916</v>
       </c>
     </row>
     <row r="46">
-      <c r="A46" t="inlineStr">
+      <c r="A46" s="2">
+        <v>45608</v>
+      </c>
+      <c r="B46" t="inlineStr">
         <is>
           <t>S26</t>
         </is>
       </c>
-      <c r="B46" t="inlineStr">
+      <c r="C46" t="inlineStr">
         <is>
           <t>T2</t>
         </is>
       </c>
-      <c r="C46" t="inlineStr">
+      <c r="D46" t="inlineStr">
         <is>
           <t>L16</t>
         </is>
       </c>
-      <c r="D46" t="inlineStr">
+      <c r="E46" t="inlineStr">
         <is>
           <t>45</t>
         </is>
       </c>
-      <c r="E46">
+      <c r="F46">
         <v>23.27</v>
       </c>
-      <c r="F46">
+      <c r="G46">
         <v>11.98</v>
       </c>
-      <c r="G46">
+      <c r="H46">
         <v>0.825</v>
       </c>
-      <c r="H46">
-        <v>0.6206137048192771</v>
+      <c r="J46">
+        <v>0.09789156626506017</v>
+      </c>
+      <c r="K46">
+        <v>1.09789156626506</v>
+      </c>
+      <c r="L46">
+        <v>0.9057605421686745</v>
       </c>
     </row>
     <row r="47">
-      <c r="A47" t="inlineStr">
+      <c r="A47" s="2">
+        <v>45608</v>
+      </c>
+      <c r="B47" t="inlineStr">
         <is>
           <t>S26</t>
         </is>
       </c>
-      <c r="B47" t="inlineStr">
+      <c r="C47" t="inlineStr">
         <is>
           <t>T2</t>
         </is>
       </c>
-      <c r="C47" t="inlineStr">
+      <c r="D47" t="inlineStr">
         <is>
           <t>L33</t>
         </is>
       </c>
-      <c r="D47" t="inlineStr">
+      <c r="E47" t="inlineStr">
         <is>
           <t>46</t>
         </is>
       </c>
-      <c r="E47">
+      <c r="F47">
         <v>10.11</v>
       </c>
-      <c r="F47">
+      <c r="G47">
         <v>5.25</v>
       </c>
-      <c r="G47">
+      <c r="H47">
         <v>1.327</v>
       </c>
-      <c r="H47">
-        <v>-0.3167612951807227</v>
+      <c r="I47" t="inlineStr">
+        <is>
+          <t>D- Extreme</t>
+        </is>
+      </c>
+      <c r="J47">
+        <v>0.6046686746987951</v>
+      </c>
+      <c r="K47">
+        <v>1.604668674698795</v>
+      </c>
+      <c r="L47">
+        <v>2.129395331325301</v>
       </c>
     </row>
     <row r="48">
-      <c r="A48" t="inlineStr">
+      <c r="A48" s="2">
+        <v>45608</v>
+      </c>
+      <c r="B48" t="inlineStr">
         <is>
           <t>S26</t>
         </is>
       </c>
-      <c r="B48" t="inlineStr">
+      <c r="C48" t="inlineStr">
         <is>
           <t>T2</t>
         </is>
       </c>
-      <c r="C48" t="inlineStr">
+      <c r="D48" t="inlineStr">
         <is>
           <t>L39</t>
         </is>
       </c>
-      <c r="D48" t="inlineStr">
+      <c r="E48" t="inlineStr">
         <is>
           <t>47</t>
         </is>
       </c>
-      <c r="E48">
+      <c r="F48">
         <v>20.85</v>
       </c>
-      <c r="F48">
+      <c r="G48">
         <v>10.47</v>
       </c>
-      <c r="G48">
+      <c r="H48">
         <v>0.615</v>
       </c>
-      <c r="H48">
-        <v>0.3505685240963857</v>
+      <c r="J48">
+        <v>0.2115963855421687</v>
+      </c>
+      <c r="K48">
+        <v>1.211596385542169</v>
+      </c>
+      <c r="L48">
+        <v>0.7451317771084338</v>
       </c>
     </row>
     <row r="49">
-      <c r="A49" t="inlineStr">
+      <c r="A49" s="2">
+        <v>45608</v>
+      </c>
+      <c r="B49" t="inlineStr">
         <is>
           <t>S26</t>
         </is>
       </c>
-      <c r="B49" t="inlineStr">
+      <c r="C49" t="inlineStr">
         <is>
           <t>T2</t>
         </is>
       </c>
-      <c r="C49" t="inlineStr">
+      <c r="D49" t="inlineStr">
         <is>
           <t>L47</t>
         </is>
       </c>
-      <c r="D49" t="inlineStr">
+      <c r="E49" t="inlineStr">
         <is>
           <t>48</t>
         </is>
       </c>
-      <c r="E49">
+      <c r="F49">
         <v>22.89</v>
       </c>
-      <c r="F49">
+      <c r="G49">
         <v>11.64</v>
       </c>
-      <c r="G49">
+      <c r="H49">
         <v>1.107</v>
       </c>
-      <c r="H49">
-        <v>0.8010745481927712</v>
+      <c r="J49">
+        <v>0.1234939759036144</v>
+      </c>
+      <c r="K49">
+        <v>1.123493975903614</v>
+      </c>
+      <c r="L49">
+        <v>1.243707831325301</v>
       </c>
     </row>
     <row r="50">
-      <c r="A50" t="inlineStr">
+      <c r="A50" s="2">
+        <v>45609</v>
+      </c>
+      <c r="B50" t="inlineStr">
         <is>
           <t>S8</t>
         </is>
       </c>
-      <c r="B50" t="inlineStr">
+      <c r="C50" t="inlineStr">
         <is>
           <t>T1</t>
         </is>
       </c>
-      <c r="C50" t="inlineStr">
+      <c r="D50" t="inlineStr">
         <is>
           <t>L3</t>
         </is>
       </c>
-      <c r="D50" t="inlineStr">
+      <c r="E50" t="inlineStr">
         <is>
           <t>49</t>
         </is>
       </c>
-      <c r="E50">
+      <c r="F50">
         <v>26.27</v>
       </c>
-      <c r="F50">
+      <c r="G50">
         <v>13.36</v>
       </c>
-      <c r="G50">
+      <c r="H50">
         <v>0.84</v>
       </c>
-      <c r="H50">
-        <v>0.8216566265060241</v>
+      <c r="J50">
+        <v>-0.006024096385542174</v>
+      </c>
+      <c r="K50">
+        <v>0.9939759036144579</v>
+      </c>
+      <c r="L50">
+        <v>0.8349397590361446</v>
       </c>
     </row>
     <row r="51">
-      <c r="A51" t="inlineStr">
+      <c r="A51" s="2">
+        <v>45609</v>
+      </c>
+      <c r="B51" t="inlineStr">
         <is>
           <t>S8</t>
         </is>
       </c>
-      <c r="B51" t="inlineStr">
+      <c r="C51" t="inlineStr">
         <is>
           <t>T1</t>
         </is>
       </c>
-      <c r="C51" t="inlineStr">
+      <c r="D51" t="inlineStr">
         <is>
           <t>L10</t>
         </is>
       </c>
-      <c r="D51" t="inlineStr">
+      <c r="E51" t="inlineStr">
         <is>
           <t>50</t>
         </is>
       </c>
-      <c r="E51">
+      <c r="F51">
         <v>26.25</v>
       </c>
-      <c r="F51">
+      <c r="G51">
         <v>13.46</v>
       </c>
-      <c r="G51">
+      <c r="H51">
         <v>1.165</v>
       </c>
-      <c r="H51">
-        <v>1.137804969879518</v>
+      <c r="J51">
+        <v>-0.01355421686746999</v>
+      </c>
+      <c r="K51">
+        <v>0.98644578313253</v>
+      </c>
+      <c r="L51">
+        <v>1.149209337349397</v>
       </c>
     </row>
     <row r="52">
-      <c r="A52" t="inlineStr">
+      <c r="A52" s="2">
+        <v>45609</v>
+      </c>
+      <c r="B52" t="inlineStr">
         <is>
           <t>S8</t>
         </is>
       </c>
-      <c r="B52" t="inlineStr">
+      <c r="C52" t="inlineStr">
         <is>
           <t>T1</t>
         </is>
       </c>
-      <c r="C52" t="inlineStr">
+      <c r="D52" t="inlineStr">
         <is>
           <t>L16</t>
         </is>
       </c>
-      <c r="D52" t="inlineStr">
+      <c r="E52" t="inlineStr">
         <is>
           <t>51</t>
         </is>
       </c>
-      <c r="E52">
+      <c r="F52">
         <v>25.72</v>
       </c>
-      <c r="F52">
+      <c r="G52">
         <v>13.1</v>
       </c>
-      <c r="G52">
+      <c r="H52">
         <v>2.288</v>
       </c>
-      <c r="H52">
-        <v>2.143277108433735</v>
+      <c r="J52">
+        <v>0.01355421686746973</v>
+      </c>
+      <c r="K52">
+        <v>1.01355421686747</v>
+      </c>
+      <c r="L52">
+        <v>2.319012048192771</v>
       </c>
     </row>
     <row r="53">
-      <c r="A53" t="inlineStr">
+      <c r="A53" s="2">
+        <v>45609</v>
+      </c>
+      <c r="B53" t="inlineStr">
         <is>
           <t>S8</t>
         </is>
       </c>
-      <c r="B53" t="inlineStr">
+      <c r="C53" t="inlineStr">
         <is>
           <t>T1</t>
         </is>
       </c>
-      <c r="C53" t="inlineStr">
+      <c r="D53" t="inlineStr">
         <is>
           <t>L33</t>
         </is>
       </c>
-      <c r="D53" t="inlineStr">
+      <c r="E53" t="inlineStr">
         <is>
           <t>52</t>
         </is>
       </c>
-      <c r="E53">
+      <c r="F53">
         <v>26.64</v>
       </c>
-      <c r="F53">
+      <c r="G53">
         <v>13.74</v>
       </c>
-      <c r="G53">
+      <c r="H53">
         <v>0.707</v>
       </c>
-      <c r="H53">
-        <v>0.7112590361445783</v>
+      <c r="I53" t="inlineStr">
+        <is>
+          <t>(dirty)</t>
+        </is>
+      </c>
+      <c r="J53">
+        <v>-0.03463855421686753</v>
+      </c>
+      <c r="K53">
+        <v>0.9653614457831324</v>
+      </c>
+      <c r="L53">
+        <v>0.6825105421686746</v>
       </c>
     </row>
     <row r="54">
-      <c r="A54" t="inlineStr">
+      <c r="A54" s="2">
+        <v>45609</v>
+      </c>
+      <c r="B54" t="inlineStr">
         <is>
           <t>S8</t>
         </is>
       </c>
-      <c r="B54" t="inlineStr">
+      <c r="C54" t="inlineStr">
         <is>
           <t>T1</t>
         </is>
       </c>
-      <c r="C54" t="inlineStr">
+      <c r="D54" t="inlineStr">
         <is>
           <t>L39</t>
         </is>
       </c>
-      <c r="D54" t="inlineStr">
+      <c r="E54" t="inlineStr">
         <is>
           <t>53</t>
         </is>
       </c>
-      <c r="E54">
+      <c r="F54">
         <v>22.04</v>
       </c>
-      <c r="F54">
+      <c r="G54">
         <v>11.21</v>
       </c>
-      <c r="G54">
+      <c r="H54">
         <v>0.287</v>
       </c>
-      <c r="H54">
-        <v>0.1893162650602409</v>
+      <c r="J54">
+        <v>0.1558734939759035</v>
+      </c>
+      <c r="K54">
+        <v>1.155873493975903</v>
+      </c>
+      <c r="L54">
+        <v>0.3317356927710843</v>
       </c>
     </row>
     <row r="55">
-      <c r="A55" t="inlineStr">
+      <c r="A55" s="2">
+        <v>45609</v>
+      </c>
+      <c r="B55" t="inlineStr">
         <is>
           <t>S8</t>
         </is>
       </c>
-      <c r="B55" t="inlineStr">
+      <c r="C55" t="inlineStr">
         <is>
           <t>T1</t>
         </is>
       </c>
-      <c r="C55" t="inlineStr">
+      <c r="D55" t="inlineStr">
         <is>
           <t>L47</t>
         </is>
       </c>
-      <c r="D55" t="inlineStr">
+      <c r="E55" t="inlineStr">
         <is>
           <t>54</t>
         </is>
       </c>
-      <c r="E55">
+      <c r="F55">
         <v>24.96</v>
       </c>
-      <c r="F55">
+      <c r="G55">
         <v>12.67</v>
       </c>
-      <c r="G55">
+      <c r="H55">
         <v>0.571</v>
       </c>
-      <c r="H55">
-        <v>0.5022048192771085</v>
+      <c r="J55">
+        <v>0.045933734939759</v>
+      </c>
+      <c r="K55">
+        <v>1.045933734939759</v>
+      </c>
+      <c r="L55">
+        <v>0.5972281626506024</v>
       </c>
     </row>
     <row r="56">
-      <c r="A56" t="inlineStr">
+      <c r="A56" s="2">
+        <v>45609</v>
+      </c>
+      <c r="B56" t="inlineStr">
         <is>
           <t>S8</t>
         </is>
       </c>
-      <c r="B56" t="inlineStr">
+      <c r="C56" t="inlineStr">
         <is>
           <t>T2</t>
         </is>
       </c>
-      <c r="C56" t="inlineStr">
+      <c r="D56" t="inlineStr">
         <is>
           <t>L3</t>
         </is>
       </c>
-      <c r="D56" t="inlineStr">
+      <c r="E56" t="inlineStr">
         <is>
           <t>55</t>
         </is>
       </c>
-      <c r="E56">
+      <c r="F56">
         <v>26.1</v>
       </c>
-      <c r="F56">
+      <c r="G56">
         <v>13.36</v>
       </c>
-      <c r="G56">
+      <c r="H56">
         <v>0.526</v>
       </c>
-      <c r="H56">
-        <v>0.5077801204819279</v>
+      <c r="J56">
+        <v>-0.006024096385542174</v>
+      </c>
+      <c r="K56">
+        <v>0.9939759036144579</v>
+      </c>
+      <c r="L56">
+        <v>0.5228313253012049</v>
       </c>
     </row>
     <row r="57">
-      <c r="A57" t="inlineStr">
+      <c r="A57" s="2">
+        <v>45609</v>
+      </c>
+      <c r="B57" t="inlineStr">
         <is>
           <t>S8</t>
         </is>
       </c>
-      <c r="B57" t="inlineStr">
+      <c r="C57" t="inlineStr">
         <is>
           <t>T2</t>
         </is>
       </c>
-      <c r="C57" t="inlineStr">
+      <c r="D57" t="inlineStr">
         <is>
           <t>L10</t>
         </is>
       </c>
-      <c r="D57" t="inlineStr">
+      <c r="E57" t="inlineStr">
         <is>
           <t>56</t>
         </is>
       </c>
-      <c r="E57">
+      <c r="F57">
         <v>26.08</v>
       </c>
-      <c r="F57">
+      <c r="G57">
         <v>13.37</v>
       </c>
-      <c r="G57">
+      <c r="H57">
         <v>0.755</v>
       </c>
-      <c r="H57">
-        <v>0.727710843373494</v>
+      <c r="J57">
+        <v>-0.006777108433735063</v>
+      </c>
+      <c r="K57">
+        <v>0.993222891566265</v>
+      </c>
+      <c r="L57">
+        <v>0.7498832831325301</v>
       </c>
     </row>
     <row r="58">
-      <c r="A58" t="inlineStr">
+      <c r="A58" s="2">
+        <v>45609</v>
+      </c>
+      <c r="B58" t="inlineStr">
         <is>
           <t>S8</t>
         </is>
       </c>
-      <c r="B58" t="inlineStr">
+      <c r="C58" t="inlineStr">
         <is>
           <t>T2</t>
         </is>
       </c>
-      <c r="C58" t="inlineStr">
+      <c r="D58" t="inlineStr">
         <is>
           <t>L16</t>
         </is>
       </c>
-      <c r="D58" t="inlineStr">
+      <c r="E58" t="inlineStr">
         <is>
           <t>57</t>
         </is>
       </c>
-      <c r="E58">
+      <c r="F58">
         <v>24.79</v>
       </c>
-      <c r="F58">
+      <c r="G58">
         <v>12.64</v>
       </c>
-      <c r="G58">
+      <c r="H58">
         <v>0.737</v>
       </c>
-      <c r="H58">
-        <v>0.6387703313253013</v>
+      <c r="J58">
+        <v>0.04819277108433726</v>
+      </c>
+      <c r="K58">
+        <v>1.048192771084337</v>
+      </c>
+      <c r="L58">
+        <v>0.7725180722891566</v>
       </c>
     </row>
     <row r="59">
-      <c r="A59" t="inlineStr">
+      <c r="A59" s="2">
+        <v>45609</v>
+      </c>
+      <c r="B59" t="inlineStr">
         <is>
           <t>S8</t>
         </is>
       </c>
-      <c r="B59" t="inlineStr">
+      <c r="C59" t="inlineStr">
         <is>
           <t>T2</t>
         </is>
       </c>
-      <c r="C59" t="inlineStr">
+      <c r="D59" t="inlineStr">
         <is>
           <t>L33</t>
         </is>
       </c>
-      <c r="D59" t="inlineStr">
+      <c r="E59" t="inlineStr">
         <is>
           <t>58</t>
         </is>
       </c>
-      <c r="E59">
+      <c r="F59">
         <v>26.64</v>
       </c>
-      <c r="F59">
+      <c r="G59">
         <v>13.31</v>
       </c>
-      <c r="G59">
+      <c r="H59">
         <v>0.124</v>
       </c>
-      <c r="H59">
-        <v>0.1247469879518072</v>
+      <c r="J59">
+        <v>-0.002259036144578399</v>
+      </c>
+      <c r="K59">
+        <v>0.9977409638554215</v>
+      </c>
+      <c r="L59">
+        <v>0.1237198795180723</v>
       </c>
     </row>
     <row r="60">
-      <c r="A60" t="inlineStr">
+      <c r="A60" s="2">
+        <v>45609</v>
+      </c>
+      <c r="B60" t="inlineStr">
         <is>
           <t>S8</t>
         </is>
       </c>
-      <c r="B60" t="inlineStr">
+      <c r="C60" t="inlineStr">
         <is>
           <t>T2</t>
         </is>
       </c>
-      <c r="C60" t="inlineStr">
+      <c r="D60" t="inlineStr">
         <is>
           <t>L39</t>
         </is>
       </c>
-      <c r="D60" t="inlineStr">
+      <c r="E60" t="inlineStr">
         <is>
           <t>59</t>
         </is>
       </c>
-      <c r="E60">
+      <c r="F60">
         <v>26.54</v>
       </c>
-      <c r="F60">
+      <c r="G60">
         <v>13.73</v>
       </c>
-      <c r="G60">
+      <c r="H60">
         <v>0.5639999999999999</v>
       </c>
-      <c r="H60">
-        <v>0.5631506024096384</v>
+      <c r="J60">
+        <v>-0.03388554216867478</v>
+      </c>
+      <c r="K60">
+        <v>0.9661144578313252</v>
+      </c>
+      <c r="L60">
+        <v>0.5448885542168673</v>
       </c>
     </row>
     <row r="61">
-      <c r="A61" t="inlineStr">
+      <c r="A61" s="2">
+        <v>45609</v>
+      </c>
+      <c r="B61" t="inlineStr">
         <is>
           <t>S8</t>
         </is>
       </c>
-      <c r="B61" t="inlineStr">
+      <c r="C61" t="inlineStr">
         <is>
           <t>T2</t>
         </is>
       </c>
-      <c r="C61" t="inlineStr">
+      <c r="D61" t="inlineStr">
         <is>
           <t>L47</t>
         </is>
       </c>
-      <c r="D61" t="inlineStr">
+      <c r="E61" t="inlineStr">
         <is>
           <t>60</t>
         </is>
       </c>
-      <c r="E61">
+      <c r="F61">
         <v>15.04</v>
       </c>
-      <c r="F61">
+      <c r="G61">
         <v>7.49</v>
       </c>
-      <c r="G61">
+      <c r="H61">
         <v>0.9</v>
       </c>
-      <c r="H61">
-        <v>0.1192771084337349</v>
+      <c r="J61">
+        <v>0.4359939759036144</v>
+      </c>
+      <c r="K61">
+        <v>1.435993975903614</v>
+      </c>
+      <c r="L61">
+        <v>1.292394578313253</v>
       </c>
     </row>
     <row r="62">
-      <c r="A62" t="inlineStr">
+      <c r="A62" s="2">
+        <v>45609</v>
+      </c>
+      <c r="B62" t="inlineStr">
         <is>
           <t>S7</t>
         </is>
       </c>
-      <c r="B62" t="inlineStr">
+      <c r="C62" t="inlineStr">
         <is>
           <t>T1</t>
         </is>
       </c>
-      <c r="C62" t="inlineStr">
+      <c r="D62" t="inlineStr">
         <is>
           <t>L3</t>
         </is>
       </c>
-      <c r="D62" t="inlineStr">
+      <c r="E62" t="inlineStr">
         <is>
           <t>61</t>
         </is>
       </c>
-      <c r="E62">
+      <c r="F62">
         <v>25.51</v>
       </c>
-      <c r="F62">
+      <c r="G62">
         <v>13.22</v>
       </c>
-      <c r="G62">
+      <c r="H62">
         <v>0.766</v>
       </c>
-      <c r="H62">
-        <v>0.7054352409638553</v>
+      <c r="J62">
+        <v>0.004518072289156664</v>
+      </c>
+      <c r="K62">
+        <v>1.004518072289157</v>
+      </c>
+      <c r="L62">
+        <v>0.7694608433734941</v>
       </c>
     </row>
     <row r="63">
-      <c r="A63" t="inlineStr">
+      <c r="A63" s="2">
+        <v>45609</v>
+      </c>
+      <c r="B63" t="inlineStr">
         <is>
           <t>S7</t>
         </is>
       </c>
-      <c r="B63" t="inlineStr">
+      <c r="C63" t="inlineStr">
         <is>
           <t>T1</t>
         </is>
       </c>
-      <c r="C63" t="inlineStr">
+      <c r="D63" t="inlineStr">
         <is>
           <t>L10</t>
         </is>
       </c>
-      <c r="D63" t="inlineStr">
+      <c r="E63" t="inlineStr">
         <is>
           <t>62</t>
         </is>
       </c>
-      <c r="E63">
+      <c r="F63">
         <v>26.29</v>
       </c>
-      <c r="F63">
+      <c r="G63">
         <v>13.62</v>
       </c>
-      <c r="G63">
+      <c r="H63">
         <v>0.805</v>
       </c>
-      <c r="H63">
-        <v>0.7886332831325302</v>
+      <c r="J63">
+        <v>-0.02560240963855434</v>
+      </c>
+      <c r="K63">
+        <v>0.9743975903614457</v>
+      </c>
+      <c r="L63">
+        <v>0.7843900602409638</v>
       </c>
     </row>
     <row r="64">
-      <c r="A64" t="inlineStr">
+      <c r="A64" s="2">
+        <v>45609</v>
+      </c>
+      <c r="B64" t="inlineStr">
         <is>
           <t>S7</t>
         </is>
       </c>
-      <c r="B64" t="inlineStr">
+      <c r="C64" t="inlineStr">
         <is>
           <t>T1</t>
         </is>
       </c>
-      <c r="C64" t="inlineStr">
+      <c r="D64" t="inlineStr">
         <is>
           <t>L16</t>
         </is>
       </c>
-      <c r="D64" t="inlineStr">
+      <c r="E64" t="inlineStr">
         <is>
           <t>63</t>
         </is>
       </c>
-      <c r="E64">
+      <c r="F64">
         <v>26.32</v>
       </c>
-      <c r="F64">
+      <c r="G64">
         <v>13.47</v>
       </c>
-      <c r="G64">
+      <c r="H64">
         <v>0.531</v>
       </c>
-      <c r="H64">
-        <v>0.5214036144578315</v>
+      <c r="J64">
+        <v>-0.01430722891566261</v>
+      </c>
+      <c r="K64">
+        <v>0.9856927710843374</v>
+      </c>
+      <c r="L64">
+        <v>0.5234028614457832</v>
       </c>
     </row>
     <row r="65">
-      <c r="A65" t="inlineStr">
+      <c r="A65" s="2">
+        <v>45609</v>
+      </c>
+      <c r="B65" t="inlineStr">
         <is>
           <t>S7</t>
         </is>
       </c>
-      <c r="B65" t="inlineStr">
+      <c r="C65" t="inlineStr">
         <is>
           <t>T1</t>
         </is>
       </c>
-      <c r="C65" t="inlineStr">
+      <c r="D65" t="inlineStr">
         <is>
           <t>L33</t>
         </is>
       </c>
-      <c r="D65" t="inlineStr">
+      <c r="E65" t="inlineStr">
         <is>
           <t>64</t>
         </is>
       </c>
-      <c r="E65">
+      <c r="F65">
         <v>26.3</v>
       </c>
-      <c r="F65">
+      <c r="G65">
         <v>13.12</v>
       </c>
-      <c r="G65">
+      <c r="H65">
         <v>1.359</v>
       </c>
-      <c r="H65">
-        <v>1.332393072289156</v>
+      <c r="J65">
+        <v>0.01204819277108421</v>
+      </c>
+      <c r="K65">
+        <v>1.012048192771084</v>
+      </c>
+      <c r="L65">
+        <v>1.375373493975903</v>
       </c>
     </row>
     <row r="66">
-      <c r="A66" t="inlineStr">
+      <c r="A66" s="2">
+        <v>45609</v>
+      </c>
+      <c r="B66" t="inlineStr">
         <is>
           <t>S7</t>
         </is>
       </c>
-      <c r="B66" t="inlineStr">
+      <c r="C66" t="inlineStr">
         <is>
           <t>T1</t>
         </is>
       </c>
-      <c r="C66" t="inlineStr">
+      <c r="D66" t="inlineStr">
         <is>
           <t>L39</t>
         </is>
       </c>
-      <c r="D66" t="inlineStr">
+      <c r="E66" t="inlineStr">
         <is>
           <t>65</t>
         </is>
       </c>
-      <c r="E66">
+      <c r="F66">
         <v>26.72</v>
       </c>
-      <c r="F66">
+      <c r="G66">
         <v>13.72</v>
       </c>
-      <c r="G66">
+      <c r="H66">
         <v>0.742</v>
       </c>
-      <c r="H66">
-        <v>0.7509397590361445</v>
+      <c r="J66">
+        <v>-0.03313253012048203</v>
+      </c>
+      <c r="K66">
+        <v>0.966867469879518</v>
+      </c>
+      <c r="L66">
+        <v>0.7174156626506023</v>
       </c>
     </row>
     <row r="67">
-      <c r="A67" t="inlineStr">
+      <c r="A67" s="2">
+        <v>45609</v>
+      </c>
+      <c r="B67" t="inlineStr">
         <is>
           <t>S7</t>
         </is>
       </c>
-      <c r="B67" t="inlineStr">
+      <c r="C67" t="inlineStr">
         <is>
           <t>T1</t>
         </is>
       </c>
-      <c r="C67" t="inlineStr">
+      <c r="D67" t="inlineStr">
         <is>
           <t>L47</t>
         </is>
       </c>
-      <c r="D67" t="inlineStr">
+      <c r="E67" t="inlineStr">
         <is>
           <t>66</t>
         </is>
       </c>
-      <c r="E67">
+      <c r="F67">
         <v>26.16</v>
       </c>
-      <c r="F67">
+      <c r="G67">
         <v>13.32</v>
       </c>
-      <c r="G67">
+      <c r="H67">
         <v>0.949</v>
       </c>
-      <c r="H67">
-        <v>0.9204156626506023</v>
+      <c r="J67">
+        <v>-0.003012048192771154</v>
+      </c>
+      <c r="K67">
+        <v>0.9969879518072289</v>
+      </c>
+      <c r="L67">
+        <v>0.9461415662650602</v>
       </c>
     </row>
     <row r="68">
-      <c r="A68" t="inlineStr">
+      <c r="A68" s="2">
+        <v>45609</v>
+      </c>
+      <c r="B68" t="inlineStr">
         <is>
           <t>S7</t>
         </is>
       </c>
-      <c r="B68" t="inlineStr">
+      <c r="C68" t="inlineStr">
         <is>
           <t>T2</t>
         </is>
       </c>
-      <c r="C68" t="inlineStr">
+      <c r="D68" t="inlineStr">
         <is>
           <t>L3</t>
         </is>
       </c>
-      <c r="D68" t="inlineStr">
+      <c r="E68" t="inlineStr">
         <is>
           <t>67</t>
         </is>
       </c>
-      <c r="E68">
+      <c r="F68">
         <v>22.23</v>
       </c>
-      <c r="F68">
+      <c r="G68">
         <v>11.18</v>
       </c>
-      <c r="G68">
+      <c r="H68">
         <v>1.757</v>
       </c>
-      <c r="H68">
-        <v>1.184122740963855</v>
+      <c r="J68">
+        <v>0.1581325301204819</v>
+      </c>
+      <c r="K68">
+        <v>1.158132530120482</v>
+      </c>
+      <c r="L68">
+        <v>2.034838855421687</v>
       </c>
     </row>
     <row r="69">
-      <c r="A69" t="inlineStr">
+      <c r="A69" s="2">
+        <v>45609</v>
+      </c>
+      <c r="B69" t="inlineStr">
         <is>
           <t>S7</t>
         </is>
       </c>
-      <c r="B69" t="inlineStr">
+      <c r="C69" t="inlineStr">
         <is>
           <t>T2</t>
         </is>
       </c>
-      <c r="C69" t="inlineStr">
+      <c r="D69" t="inlineStr">
         <is>
           <t>L10</t>
         </is>
       </c>
-      <c r="D69" t="inlineStr">
+      <c r="E69" t="inlineStr">
         <is>
           <t>68</t>
         </is>
       </c>
-      <c r="E69">
+      <c r="F69">
         <v>25.52</v>
       </c>
-      <c r="F69">
+      <c r="G69">
         <v>12.95</v>
       </c>
-      <c r="G69">
+      <c r="H69">
         <v>2.094</v>
       </c>
-      <c r="H69">
-        <v>1.930012048192772</v>
+      <c r="J69">
+        <v>0.02484939759036145</v>
+      </c>
+      <c r="K69">
+        <v>1.024849397590361</v>
+      </c>
+      <c r="L69">
+        <v>2.146034638554217</v>
       </c>
     </row>
     <row r="70">
-      <c r="A70" t="inlineStr">
+      <c r="A70" s="2">
+        <v>45609</v>
+      </c>
+      <c r="B70" t="inlineStr">
         <is>
           <t>S7</t>
         </is>
       </c>
-      <c r="B70" t="inlineStr">
+      <c r="C70" t="inlineStr">
         <is>
           <t>T2</t>
         </is>
       </c>
-      <c r="C70" t="inlineStr">
+      <c r="D70" t="inlineStr">
         <is>
           <t>L16</t>
         </is>
       </c>
-      <c r="D70" t="inlineStr">
+      <c r="E70" t="inlineStr">
         <is>
           <t>69</t>
         </is>
       </c>
-      <c r="E70">
+      <c r="F70">
         <v>26.45</v>
       </c>
-      <c r="F70">
+      <c r="G70">
         <v>13.63</v>
       </c>
-      <c r="G70">
+      <c r="H70">
         <v>0.778</v>
       </c>
-      <c r="H70">
-        <v>0.7715557228915663</v>
+      <c r="J70">
+        <v>-0.02635542168674696</v>
+      </c>
+      <c r="K70">
+        <v>0.973644578313253</v>
+      </c>
+      <c r="L70">
+        <v>0.7574954819277109</v>
       </c>
     </row>
     <row r="71">
-      <c r="A71" t="inlineStr">
+      <c r="A71" s="2">
+        <v>45609</v>
+      </c>
+      <c r="B71" t="inlineStr">
         <is>
           <t>S7</t>
         </is>
       </c>
-      <c r="B71" t="inlineStr">
+      <c r="C71" t="inlineStr">
         <is>
           <t>T2</t>
         </is>
       </c>
-      <c r="C71" t="inlineStr">
+      <c r="D71" t="inlineStr">
         <is>
           <t>L33</t>
         </is>
       </c>
-      <c r="D71" t="inlineStr">
+      <c r="E71" t="inlineStr">
         <is>
           <t>70</t>
         </is>
       </c>
-      <c r="E71">
+      <c r="F71">
         <v>26.82</v>
       </c>
-      <c r="F71">
+      <c r="G71">
         <v>13.69</v>
       </c>
-      <c r="G71">
+      <c r="H71">
         <v>0.5610000000000001</v>
       </c>
-      <c r="H71">
-        <v>0.5719834337349399</v>
+      <c r="J71">
+        <v>-0.03087349397590363</v>
+      </c>
+      <c r="K71">
+        <v>0.9691265060240963</v>
+      </c>
+      <c r="L71">
+        <v>0.5436799698795181</v>
       </c>
     </row>
     <row r="72">
-      <c r="A72" t="inlineStr">
+      <c r="A72" s="2">
+        <v>45609</v>
+      </c>
+      <c r="B72" t="inlineStr">
         <is>
           <t>S7</t>
         </is>
       </c>
-      <c r="B72" t="inlineStr">
+      <c r="C72" t="inlineStr">
         <is>
           <t>T2</t>
         </is>
       </c>
-      <c r="C72" t="inlineStr">
+      <c r="D72" t="inlineStr">
         <is>
           <t>L39</t>
         </is>
       </c>
-      <c r="D72" t="inlineStr">
+      <c r="E72" t="inlineStr">
         <is>
           <t>71</t>
         </is>
       </c>
-      <c r="E72">
+      <c r="F72">
         <v>26.09</v>
       </c>
-      <c r="F72">
+      <c r="G72">
         <v>13.18</v>
       </c>
-      <c r="G72">
+      <c r="H72">
         <v>0.31</v>
       </c>
-      <c r="H72">
-        <v>0.2990286144578314</v>
+      <c r="J72">
+        <v>0.007530120481927685</v>
+      </c>
+      <c r="K72">
+        <v>1.007530120481928</v>
+      </c>
+      <c r="L72">
+        <v>0.3123343373493975</v>
       </c>
     </row>
     <row r="73">
-      <c r="A73" t="inlineStr">
+      <c r="A73" s="2">
+        <v>45609</v>
+      </c>
+      <c r="B73" t="inlineStr">
         <is>
           <t>S7</t>
         </is>
       </c>
-      <c r="B73" t="inlineStr">
+      <c r="C73" t="inlineStr">
         <is>
           <t>T2</t>
         </is>
       </c>
-      <c r="C73" t="inlineStr">
+      <c r="D73" t="inlineStr">
         <is>
           <t>L47</t>
         </is>
       </c>
-      <c r="D73" t="inlineStr">
+      <c r="E73" t="inlineStr">
         <is>
           <t>72</t>
         </is>
       </c>
-      <c r="E73">
+      <c r="F73">
         <v>26.9</v>
       </c>
-      <c r="F73">
+      <c r="G73">
         <v>13.84</v>
       </c>
-      <c r="G73">
+      <c r="H73">
         <v>1.638</v>
       </c>
-      <c r="H73">
-        <v>1.679936746987952</v>
+      <c r="J73">
+        <v>-0.04216867469879522</v>
+      </c>
+      <c r="K73">
+        <v>0.9578313253012047</v>
+      </c>
+      <c r="L73">
+        <v>1.568927710843373</v>
       </c>
     </row>
   </sheetData>

</xml_diff>